<commit_message>
Some fixes and refactoring.
</commit_message>
<xml_diff>
--- a/src/main/resources/result.xlsx
+++ b/src/main/resources/result.xlsx
@@ -199,21 +199,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
+    <col min="3" max="3" width="10.16796875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="5.734375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="9.65625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="4.6875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.16796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="8.7265625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="5.734375" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="31.9140625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="8.31640625" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="11.3203125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="28.1171875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.66796875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="31.9140625" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="19.48046875" customWidth="true" bestFit="true"/>
-    <col min="1" max="1" width="9.65625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="28.1171875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="15.47265625" customWidth="true" bestFit="true"/>
     <col min="15" max="15" width="9.671875" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="11.3203125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="23.453125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="31.7265625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="15.47265625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="8.31640625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="23.453125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="25.5546875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Bugs with cancel fixed. Added an example of console app
</commit_message>
<xml_diff>
--- a/src/main/resources/result.xlsx
+++ b/src/main/resources/result.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Фамилия</t>
   </si>
@@ -516,8 +516,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="D2" s="0" t="s">
-        <v>18</v>
+      <c r="A2" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>